<commit_message>
Switched to using file-samples for unit-tests.
</commit_message>
<xml_diff>
--- a/tests/samples/budget.xlsx
+++ b/tests/samples/budget.xlsx
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
   <si>
     <t>Salary</t>
@@ -50,9 +53,6 @@
   </si>
   <si>
     <t>Party</t>
-  </si>
-  <si>
-    <t>Cash</t>
   </si>
   <si>
     <t>DAILY</t>
@@ -227,17 +227,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N63" totalsRowCount="1">
   <tableColumns count="14">
     <tableColumn id="1" name="DATE" totalsRowLabel="TOTALS" dataDxfId="0"/>
-    <tableColumn id="2" name="Salary" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="3" name="Rent" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="4" name="WaterBill" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="5" name="PowerBill" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="6" name="PhoneBill" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="7" name="Food" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="8" name="Commute" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="9" name="Tobacco" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="10" name="Snacks" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="11" name="Party" totalsRowFunction="sum" dataDxfId="1"/>
-    <tableColumn id="12" name="Cash" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="2" name="Cash" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="3" name="Salary" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="4" name="Rent" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="5" name="WaterBill" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="6" name="PowerBill" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="7" name="PhoneBill" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="8" name="Food" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="9" name="Commute" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="10" name="Tobacco" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="11" name="Snacks" totalsRowFunction="sum" dataDxfId="1"/>
+    <tableColumn id="12" name="Party" totalsRowFunction="sum" dataDxfId="1"/>
     <tableColumn id="13" name="DAILY" dataDxfId="2"/>
     <tableColumn id="14" name="CUMULATIVE" dataDxfId="3"/>
   </tableColumns>
@@ -542,17 +542,17 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
   </cols>
@@ -606,7 +606,7 @@
         <v>44136</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -621,22 +621,22 @@
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I2" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J2" s="3">
+        <v>-15</v>
+      </c>
+      <c r="K2" s="3">
         <v>-10</v>
       </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
       <c r="L2" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M2" s="4">
         <f>SUM(B2:L2)</f>
@@ -667,13 +667,13 @@
         <v>0</v>
       </c>
       <c r="G3" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I3" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -698,11 +698,11 @@
         <v>44138</v>
       </c>
       <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
         <v>1300</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
@@ -713,13 +713,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I4" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J4" s="3">
         <v>0</v>
@@ -759,19 +759,19 @@
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
         <v>-10</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
@@ -805,13 +805,13 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I6" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -848,16 +848,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>-25</v>
       </c>
-      <c r="G7" s="3">
-        <v>-15</v>
-      </c>
       <c r="H7" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I7" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J7" s="3">
         <v>0</v>
@@ -891,25 +891,25 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <v>-60</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
       <c r="G8" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H8" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
         <v>-10</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
       </c>
       <c r="L8" s="3">
         <v>0</v>
@@ -934,25 +934,25 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
         <v>-30</v>
       </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
       <c r="F9" s="3">
         <v>0</v>
       </c>
       <c r="G9" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H9" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I9" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K9" s="3">
         <v>0</v>
@@ -989,13 +989,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H10" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
@@ -1035,19 +1035,19 @@
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H11" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I11" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
         <v>-10</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
       </c>
       <c r="L11" s="3">
         <v>0</v>
@@ -1081,13 +1081,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I12" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
@@ -1127,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H13" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I13" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J13" s="3">
         <v>0</v>
@@ -1173,22 +1173,22 @@
         <v>0</v>
       </c>
       <c r="G14" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I14" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
         <v>-10</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>-20</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0</v>
       </c>
       <c r="M14" s="4">
         <f>SUM(B14:L14)</f>
@@ -1219,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
@@ -1231,10 +1231,10 @@
         <v>0</v>
       </c>
       <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
         <v>-20</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(B15:L15)</f>
@@ -1253,11 +1253,11 @@
         <v>0</v>
       </c>
       <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
         <v>-450</v>
       </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
@@ -1265,16 +1265,16 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H16" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I16" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J16" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
@@ -1311,19 +1311,19 @@
         <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H17" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I17" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
         <v>-10</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -1357,13 +1357,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H18" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I18" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J18" s="3">
         <v>0</v>
@@ -1403,13 +1403,13 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H19" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I19" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
@@ -1449,19 +1449,19 @@
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H20" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I20" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
         <v>-10</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
       </c>
       <c r="L20" s="3">
         <v>0</v>
@@ -1495,13 +1495,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I21" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J21" s="3">
         <v>0</v>
@@ -1541,10 +1541,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
@@ -1587,19 +1587,19 @@
         <v>0</v>
       </c>
       <c r="G23" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I23" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J23" s="3">
+        <v>-15</v>
+      </c>
+      <c r="K23" s="3">
         <v>-10</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>
@@ -1633,13 +1633,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H24" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I24" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J24" s="3">
         <v>0</v>
@@ -1679,13 +1679,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H25" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I25" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J25" s="3">
         <v>0</v>
@@ -1725,19 +1725,19 @@
         <v>0</v>
       </c>
       <c r="G26" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H26" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I26" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
         <v>-10</v>
-      </c>
-      <c r="K26" s="3">
-        <v>0</v>
       </c>
       <c r="L26" s="3">
         <v>0</v>
@@ -1771,13 +1771,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H27" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I27" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J27" s="3">
         <v>0</v>
@@ -1817,22 +1817,22 @@
         <v>0</v>
       </c>
       <c r="G28" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H28" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I28" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J28" s="3">
         <v>0</v>
       </c>
       <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
         <v>-20</v>
-      </c>
-      <c r="L28" s="3">
-        <v>0</v>
       </c>
       <c r="M28" s="4">
         <f>SUM(B28:L28)</f>
@@ -1863,22 +1863,22 @@
         <v>0</v>
       </c>
       <c r="G29" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I29" s="3">
         <v>0</v>
       </c>
       <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
         <v>-10</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="3">
         <v>-20</v>
-      </c>
-      <c r="L29" s="3">
-        <v>0</v>
       </c>
       <c r="M29" s="4">
         <f>SUM(B29:L29)</f>
@@ -1909,16 +1909,16 @@
         <v>0</v>
       </c>
       <c r="G30" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I30" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J30" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K30" s="3">
         <v>0</v>
@@ -1955,13 +1955,13 @@
         <v>0</v>
       </c>
       <c r="G31" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H31" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I31" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J31" s="3">
         <v>0</v>
@@ -2001,19 +2001,19 @@
         <v>0</v>
       </c>
       <c r="G32" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H32" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I32" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
         <v>-10</v>
-      </c>
-      <c r="K32" s="3">
-        <v>0</v>
       </c>
       <c r="L32" s="3">
         <v>0</v>
@@ -2047,13 +2047,13 @@
         <v>0</v>
       </c>
       <c r="G33" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H33" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I33" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J33" s="3">
         <v>0</v>
@@ -2078,11 +2078,11 @@
         <v>44168</v>
       </c>
       <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3">
         <v>1300</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
       <c r="D34" s="3">
         <v>0</v>
       </c>
@@ -2093,13 +2093,13 @@
         <v>0</v>
       </c>
       <c r="G34" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H34" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J34" s="3">
         <v>0</v>
@@ -2139,19 +2139,19 @@
         <v>0</v>
       </c>
       <c r="G35" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H35" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I35" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
         <v>-10</v>
-      </c>
-      <c r="K35" s="3">
-        <v>0</v>
       </c>
       <c r="L35" s="3">
         <v>0</v>
@@ -2185,10 +2185,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H36" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
@@ -2228,19 +2228,19 @@
         <v>0</v>
       </c>
       <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
         <v>-25</v>
       </c>
-      <c r="G37" s="3">
-        <v>-15</v>
-      </c>
       <c r="H37" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I37" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J37" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
@@ -2271,25 +2271,25 @@
         <v>0</v>
       </c>
       <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
         <v>-60</v>
       </c>
-      <c r="F38" s="3">
-        <v>0</v>
-      </c>
       <c r="G38" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H38" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I38" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
         <v>-10</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0</v>
       </c>
       <c r="L38" s="3">
         <v>0</v>
@@ -2314,22 +2314,22 @@
         <v>0</v>
       </c>
       <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
         <v>-30</v>
       </c>
-      <c r="E39" s="3">
-        <v>0</v>
-      </c>
       <c r="F39" s="3">
         <v>0</v>
       </c>
       <c r="G39" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H39" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J39" s="3">
         <v>0</v>
@@ -2369,13 +2369,13 @@
         <v>0</v>
       </c>
       <c r="G40" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H40" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I40" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J40" s="3">
         <v>0</v>
@@ -2415,19 +2415,19 @@
         <v>0</v>
       </c>
       <c r="G41" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H41" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I41" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
         <v>-10</v>
-      </c>
-      <c r="K41" s="3">
-        <v>0</v>
       </c>
       <c r="L41" s="3">
         <v>0</v>
@@ -2461,22 +2461,22 @@
         <v>0</v>
       </c>
       <c r="G42" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H42" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I42" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J42" s="3">
         <v>0</v>
       </c>
       <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
         <v>-20</v>
-      </c>
-      <c r="L42" s="3">
-        <v>0</v>
       </c>
       <c r="M42" s="4">
         <f>SUM(B42:L42)</f>
@@ -2507,10 +2507,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H43" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I43" s="3">
         <v>0</v>
@@ -2519,10 +2519,10 @@
         <v>0</v>
       </c>
       <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
         <v>-20</v>
-      </c>
-      <c r="L43" s="3">
-        <v>0</v>
       </c>
       <c r="M43" s="4">
         <f>SUM(B43:L43)</f>
@@ -2553,19 +2553,19 @@
         <v>0</v>
       </c>
       <c r="G44" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H44" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I44" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J44" s="3">
+        <v>-15</v>
+      </c>
+      <c r="K44" s="3">
         <v>-10</v>
-      </c>
-      <c r="K44" s="3">
-        <v>0</v>
       </c>
       <c r="L44" s="3">
         <v>0</v>
@@ -2599,13 +2599,13 @@
         <v>0</v>
       </c>
       <c r="G45" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H45" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I45" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J45" s="3">
         <v>0</v>
@@ -2633,11 +2633,11 @@
         <v>0</v>
       </c>
       <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
         <v>-450</v>
       </c>
-      <c r="D46" s="3">
-        <v>0</v>
-      </c>
       <c r="E46" s="3">
         <v>0</v>
       </c>
@@ -2645,13 +2645,13 @@
         <v>0</v>
       </c>
       <c r="G46" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H46" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I46" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J46" s="3">
         <v>0</v>
@@ -2691,19 +2691,19 @@
         <v>0</v>
       </c>
       <c r="G47" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H47" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3">
         <v>-10</v>
-      </c>
-      <c r="K47" s="3">
-        <v>0</v>
       </c>
       <c r="L47" s="3">
         <v>0</v>
@@ -2737,13 +2737,13 @@
         <v>0</v>
       </c>
       <c r="G48" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H48" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I48" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J48" s="3">
         <v>0</v>
@@ -2783,13 +2783,13 @@
         <v>0</v>
       </c>
       <c r="G49" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H49" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I49" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J49" s="3">
         <v>0</v>
@@ -2829,19 +2829,19 @@
         <v>0</v>
       </c>
       <c r="G50" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H50" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I50" s="3">
         <v>0</v>
       </c>
       <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
         <v>-10</v>
-      </c>
-      <c r="K50" s="3">
-        <v>0</v>
       </c>
       <c r="L50" s="3">
         <v>0</v>
@@ -2875,16 +2875,16 @@
         <v>0</v>
       </c>
       <c r="G51" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H51" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I51" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J51" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K51" s="3">
         <v>0</v>
@@ -2921,13 +2921,13 @@
         <v>0</v>
       </c>
       <c r="G52" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H52" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I52" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J52" s="3">
         <v>0</v>
@@ -2967,19 +2967,19 @@
         <v>0</v>
       </c>
       <c r="G53" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H53" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I53" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J53" s="3">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
         <v>-10</v>
-      </c>
-      <c r="K53" s="3">
-        <v>0</v>
       </c>
       <c r="L53" s="3">
         <v>0</v>
@@ -3013,13 +3013,13 @@
         <v>0</v>
       </c>
       <c r="G54" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H54" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I54" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J54" s="3">
         <v>0</v>
@@ -3059,13 +3059,13 @@
         <v>0</v>
       </c>
       <c r="G55" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H55" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I55" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J55" s="3">
         <v>0</v>
@@ -3105,22 +3105,22 @@
         <v>0</v>
       </c>
       <c r="G56" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H56" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I56" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
         <v>-10</v>
       </c>
-      <c r="K56" s="3">
+      <c r="L56" s="3">
         <v>-20</v>
-      </c>
-      <c r="L56" s="3">
-        <v>0</v>
       </c>
       <c r="M56" s="4">
         <f>SUM(B56:L56)</f>
@@ -3151,10 +3151,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H57" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I57" s="3">
         <v>0</v>
@@ -3163,10 +3163,10 @@
         <v>0</v>
       </c>
       <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3">
         <v>-20</v>
-      </c>
-      <c r="L57" s="3">
-        <v>0</v>
       </c>
       <c r="M57" s="4">
         <f>SUM(B57:L57)</f>
@@ -3197,16 +3197,16 @@
         <v>0</v>
       </c>
       <c r="G58" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H58" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="I58" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J58" s="3">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="K58" s="3">
         <v>0</v>
@@ -3243,19 +3243,19 @@
         <v>0</v>
       </c>
       <c r="G59" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H59" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I59" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
         <v>-10</v>
-      </c>
-      <c r="K59" s="3">
-        <v>0</v>
       </c>
       <c r="L59" s="3">
         <v>0</v>
@@ -3289,13 +3289,13 @@
         <v>0</v>
       </c>
       <c r="G60" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H60" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I60" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J60" s="3">
         <v>0</v>
@@ -3335,13 +3335,13 @@
         <v>0</v>
       </c>
       <c r="G61" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H61" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I61" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J61" s="3">
         <v>0</v>
@@ -3381,19 +3381,19 @@
         <v>0</v>
       </c>
       <c r="G62" s="3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H62" s="3">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="I62" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
         <v>-10</v>
-      </c>
-      <c r="K62" s="3">
-        <v>0</v>
       </c>
       <c r="L62" s="3">
         <v>0</v>
@@ -3412,47 +3412,47 @@
         <v>0</v>
       </c>
       <c r="B63" s="3">
+        <f>SUBTOTAL(109,[Cash])</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="3">
         <f>SUBTOTAL(109,[Salary])</f>
         <v>0</v>
       </c>
-      <c r="C63" s="3">
+      <c r="D63" s="3">
         <f>SUBTOTAL(109,[Rent])</f>
         <v>0</v>
       </c>
-      <c r="D63" s="3">
+      <c r="E63" s="3">
         <f>SUBTOTAL(109,[WaterBill])</f>
         <v>0</v>
       </c>
-      <c r="E63" s="3">
+      <c r="F63" s="3">
         <f>SUBTOTAL(109,[PowerBill])</f>
         <v>0</v>
       </c>
-      <c r="F63" s="3">
+      <c r="G63" s="3">
         <f>SUBTOTAL(109,[PhoneBill])</f>
         <v>0</v>
       </c>
-      <c r="G63" s="3">
+      <c r="H63" s="3">
         <f>SUBTOTAL(109,[Food])</f>
         <v>0</v>
       </c>
-      <c r="H63" s="3">
+      <c r="I63" s="3">
         <f>SUBTOTAL(109,[Commute])</f>
         <v>0</v>
       </c>
-      <c r="I63" s="3">
+      <c r="J63" s="3">
         <f>SUBTOTAL(109,[Tobacco])</f>
         <v>0</v>
       </c>
-      <c r="J63" s="3">
+      <c r="K63" s="3">
         <f>SUBTOTAL(109,[Snacks])</f>
         <v>0</v>
       </c>
-      <c r="K63" s="3">
+      <c r="L63" s="3">
         <f>SUBTOTAL(109,[Party])</f>
-        <v>0</v>
-      </c>
-      <c r="L63" s="3">
-        <f>SUBTOTAL(109,[Cash])</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>